<commit_message>
JK: order report list
</commit_message>
<xml_diff>
--- a/modules/jk/files/excel_example.xlsx
+++ b/modules/jk/files/excel_example.xlsx
@@ -1383,11 +1383,11 @@
   <dimension ref="A1:AMJ159"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E5" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
JK: #HRCENTER-171 update xls-file
</commit_message>
<xml_diff>
--- a/modules/jk/files/excel_example.xlsx
+++ b/modules/jk/files/excel_example.xlsx
@@ -1000,13 +1000,9 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1198,11 +1194,11 @@
   <dimension ref="A1:AMJ159"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="BK4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="BK1" activeCellId="0" sqref="BK1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1228,1273 +1224,1273 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="40" min="38" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="53" min="42" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="2" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="3" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="2" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="58" style="3" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="2" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="61" style="3" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="3" width="34.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="3" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="3" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="66" style="3" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="2" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="58" style="2" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="61" style="2" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="2" width="34.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="2" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="2" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="66" style="2" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="80" min="69" style="4" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="81" style="5" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="6" width="9.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="80" min="69" style="3" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="81" style="4" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="5" width="9.15"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="9" customFormat="true" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8" t="s">
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8" t="s">
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
-      <c r="AW1" s="8"/>
-      <c r="AX1" s="8" t="s">
+      <c r="AS1" s="7"/>
+      <c r="AT1" s="7"/>
+      <c r="AU1" s="7"/>
+      <c r="AV1" s="7"/>
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="AY1" s="8"/>
-      <c r="AZ1" s="8"/>
-      <c r="BA1" s="8"/>
-      <c r="BB1" s="8" t="s">
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BC1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BD1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BE1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="BF1" s="8" t="s">
+      <c r="BF1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BG1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BH1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BI1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="BJ1" s="8" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="BK1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="BL1" s="8" t="s">
+      <c r="BL1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BM1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BN1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="BO1" s="8"/>
-      <c r="BP1" s="8" t="s">
+      <c r="BO1" s="7"/>
+      <c r="BP1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="BQ1" s="9"/>
-      <c r="BR1" s="9"/>
-      <c r="BS1" s="9"/>
-      <c r="BT1" s="9"/>
-      <c r="BU1" s="9"/>
-      <c r="BV1" s="9"/>
-      <c r="BW1" s="9"/>
-      <c r="BX1" s="9"/>
-      <c r="BY1" s="9"/>
-      <c r="BZ1" s="9"/>
-      <c r="CA1" s="9"/>
-      <c r="CB1" s="9"/>
-      <c r="AMJ1" s="11"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="AMJ1" s="10"/>
     </row>
-    <row r="2" s="10" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7" t="s">
+    <row r="2" s="9" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="8" t="s">
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AH2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AI2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AJ2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AK2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AL2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AM2" s="8" t="s">
+      <c r="AM2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AN2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AO2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AQ2" s="8" t="s">
+      <c r="AQ2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AR2" s="8" t="s">
+      <c r="AR2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AS2" s="13" t="s">
+      <c r="AS2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="AT2" s="13" t="s">
+      <c r="AT2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="AU2" s="8" t="s">
+      <c r="AU2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AV2" s="8" t="s">
+      <c r="AV2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="14" t="s">
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AY2" s="8" t="s">
+      <c r="AY2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AZ2" s="8" t="s">
+      <c r="AZ2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="BA2" s="8" t="s">
+      <c r="BA2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="BB2" s="8"/>
-      <c r="BC2" s="8"/>
-      <c r="BD2" s="8"/>
-      <c r="BE2" s="8"/>
-      <c r="BF2" s="8"/>
-      <c r="BG2" s="8"/>
-      <c r="BH2" s="8"/>
-      <c r="BI2" s="8"/>
-      <c r="BJ2" s="8"/>
-      <c r="BK2" s="8"/>
-      <c r="BL2" s="8"/>
-      <c r="BM2" s="8"/>
-      <c r="BN2" s="8" t="s">
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="7"/>
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="7"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="7"/>
+      <c r="BH2" s="7"/>
+      <c r="BI2" s="7"/>
+      <c r="BJ2" s="7"/>
+      <c r="BK2" s="7"/>
+      <c r="BL2" s="7"/>
+      <c r="BM2" s="7"/>
+      <c r="BN2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="BO2" s="8" t="s">
+      <c r="BO2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="BP2" s="8"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="9"/>
-      <c r="BS2" s="9"/>
-      <c r="BT2" s="9"/>
-      <c r="BU2" s="9"/>
-      <c r="BV2" s="9"/>
-      <c r="BW2" s="9"/>
-      <c r="BX2" s="9"/>
-      <c r="BY2" s="9"/>
-      <c r="BZ2" s="9"/>
-      <c r="CA2" s="9"/>
-      <c r="CB2" s="9"/>
-      <c r="AMJ2" s="11"/>
+      <c r="BP2" s="7"/>
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="8"/>
+      <c r="CB2" s="8"/>
+      <c r="AMJ2" s="10"/>
     </row>
-    <row r="3" s="10" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="8"/>
-      <c r="AL3" s="8"/>
-      <c r="AM3" s="8"/>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8"/>
-      <c r="AP3" s="7"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="13"/>
-      <c r="AT3" s="13"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="13" t="s">
+    <row r="3" s="9" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7"/>
+      <c r="AM3" s="7"/>
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="12"/>
+      <c r="AT3" s="12"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AW3" s="8" t="s">
+      <c r="AW3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AX3" s="14"/>
-      <c r="AY3" s="8"/>
-      <c r="AZ3" s="8"/>
-      <c r="BA3" s="8"/>
-      <c r="BB3" s="8"/>
-      <c r="BC3" s="8"/>
-      <c r="BD3" s="8"/>
-      <c r="BE3" s="8"/>
-      <c r="BF3" s="8"/>
-      <c r="BG3" s="8"/>
-      <c r="BH3" s="8"/>
-      <c r="BI3" s="8"/>
-      <c r="BJ3" s="8"/>
-      <c r="BK3" s="8"/>
-      <c r="BL3" s="8"/>
-      <c r="BM3" s="8"/>
-      <c r="BN3" s="8"/>
-      <c r="BO3" s="8"/>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="9"/>
-      <c r="BR3" s="9"/>
-      <c r="BS3" s="9"/>
-      <c r="BT3" s="9"/>
-      <c r="BU3" s="9"/>
-      <c r="BV3" s="9"/>
-      <c r="BW3" s="9"/>
-      <c r="BX3" s="9"/>
-      <c r="BY3" s="9"/>
-      <c r="BZ3" s="9"/>
-      <c r="CA3" s="9"/>
-      <c r="CB3" s="9"/>
-      <c r="AMJ3" s="11"/>
+      <c r="AX3" s="13"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
+      <c r="BA3" s="7"/>
+      <c r="BB3" s="7"/>
+      <c r="BC3" s="7"/>
+      <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
+      <c r="BF3" s="7"/>
+      <c r="BG3" s="7"/>
+      <c r="BH3" s="7"/>
+      <c r="BI3" s="7"/>
+      <c r="BJ3" s="7"/>
+      <c r="BK3" s="7"/>
+      <c r="BL3" s="7"/>
+      <c r="BM3" s="7"/>
+      <c r="BN3" s="7"/>
+      <c r="BO3" s="7"/>
+      <c r="BP3" s="7"/>
+      <c r="BQ3" s="8"/>
+      <c r="BR3" s="8"/>
+      <c r="BS3" s="8"/>
+      <c r="BT3" s="8"/>
+      <c r="BU3" s="8"/>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8"/>
+      <c r="CA3" s="8"/>
+      <c r="CB3" s="8"/>
+      <c r="AMJ3" s="10"/>
     </row>
-    <row r="4" s="24" customFormat="true" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="n">
+    <row r="4" s="23" customFormat="true" ht="52.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="N4" s="15" t="n">
+      <c r="N4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="P4" s="15" t="n">
+      <c r="P4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="R4" s="15" t="s">
+      <c r="R4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="S4" s="15" t="n">
+      <c r="S4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="U4" s="15" t="s">
+      <c r="U4" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="X4" s="15" t="n">
+      <c r="X4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="Y4" s="15" t="s">
+      <c r="Y4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="Z4" s="15" t="s">
+      <c r="Z4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="AA4" s="15" t="s">
+      <c r="AA4" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AB4" s="15" t="n">
+      <c r="AB4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="AC4" s="18" t="s">
+      <c r="AC4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AD4" s="18" t="s">
+      <c r="AD4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AE4" s="18" t="n">
+      <c r="AE4" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="AF4" s="18" t="s">
+      <c r="AF4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AG4" s="19" t="s">
+      <c r="AG4" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="AH4" s="19"/>
-      <c r="AI4" s="19" t="n">
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18" t="n">
         <v>0.2</v>
       </c>
-      <c r="AJ4" s="19" t="n">
+      <c r="AJ4" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="AK4" s="19" t="n">
+      <c r="AK4" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="AL4" s="19" t="s">
+      <c r="AL4" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="AM4" s="19" t="s">
+      <c r="AM4" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="AN4" s="19" t="s">
+      <c r="AN4" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="AO4" s="19" t="n">
+      <c r="AO4" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="AP4" s="15" t="s">
+      <c r="AP4" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AQ4" s="15" t="n">
+      <c r="AQ4" s="14" t="n">
         <v>35</v>
       </c>
-      <c r="AR4" s="15" t="s">
+      <c r="AR4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="AS4" s="20" t="s">
+      <c r="AS4" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AT4" s="20" t="s">
+      <c r="AT4" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AU4" s="21" t="e">
+      <c r="AU4" s="20" t="e">
         <f aca="false">IF(AQ4/(AR4-AT4/AS4*AR4)&gt;=1,1,AQ4/(AR4-AT4/AS4*AR4))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AV4" s="20" t="s">
+      <c r="AV4" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AW4" s="20" t="s">
+      <c r="AW4" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="AX4" s="18" t="s">
+      <c r="AX4" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AY4" s="15" t="s">
+      <c r="AY4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="AZ4" s="15" t="s">
+      <c r="AZ4" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="BA4" s="15" t="s">
+      <c r="BA4" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="BB4" s="21" t="n">
+      <c r="BB4" s="20" t="n">
         <f aca="false">AO4+AK4+AE4+AB4+X4+S4+P4+N4</f>
         <v>8</v>
       </c>
-      <c r="BC4" s="15" t="s">
+      <c r="BC4" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="BD4" s="15" t="s">
+      <c r="BD4" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="BE4" s="15" t="s">
+      <c r="BE4" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="BF4" s="15" t="s">
+      <c r="BF4" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="BG4" s="15" t="s">
+      <c r="BG4" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="BH4" s="15" t="s">
+      <c r="BH4" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="BI4" s="15" t="s">
+      <c r="BI4" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="BJ4" s="15" t="s">
+      <c r="BJ4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="BK4" s="15" t="s">
+      <c r="BK4" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="BL4" s="15" t="s">
+      <c r="BL4" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="BM4" s="22" t="s">
+      <c r="BM4" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="BN4" s="18" t="s">
+      <c r="BN4" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="BO4" s="21" t="s">
+      <c r="BO4" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="BP4" s="18" t="s">
+      <c r="BP4" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="BQ4" s="23"/>
-      <c r="BR4" s="23"/>
-      <c r="BS4" s="23"/>
-      <c r="BT4" s="23"/>
-      <c r="BU4" s="23"/>
-      <c r="BV4" s="23"/>
-      <c r="BW4" s="23"/>
-      <c r="BX4" s="23"/>
-      <c r="BY4" s="23"/>
-      <c r="BZ4" s="23"/>
-      <c r="CA4" s="23"/>
-      <c r="CB4" s="23"/>
-      <c r="AMJ4" s="25"/>
+      <c r="BQ4" s="22"/>
+      <c r="BR4" s="22"/>
+      <c r="BS4" s="22"/>
+      <c r="BT4" s="22"/>
+      <c r="BU4" s="22"/>
+      <c r="BV4" s="22"/>
+      <c r="BW4" s="22"/>
+      <c r="BX4" s="22"/>
+      <c r="BY4" s="22"/>
+      <c r="BZ4" s="22"/>
+      <c r="CA4" s="22"/>
+      <c r="CB4" s="22"/>
+      <c r="AMJ4" s="24"/>
     </row>
-    <row r="5" s="15" customFormat="true" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+    <row r="5" s="14" customFormat="true" ht="52.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="P5" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="S5" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="U5" s="15" t="s">
+      <c r="U5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="V5" s="15" t="s">
+      <c r="V5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="W5" s="15" t="s">
+      <c r="W5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="X5" s="15" t="s">
+      <c r="X5" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="Y5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="Z5" s="15" t="s">
+      <c r="Z5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AA5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AB5" s="15" t="s">
+      <c r="AB5" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="AC5" s="15" t="s">
+      <c r="AC5" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="AD5" s="15" t="s">
+      <c r="AD5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="AE5" s="15" t="s">
+      <c r="AE5" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="AF5" s="15" t="s">
+      <c r="AF5" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="AG5" s="15" t="s">
+      <c r="AG5" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="AH5" s="15" t="s">
+      <c r="AH5" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AI5" s="15" t="s">
+      <c r="AI5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AJ5" s="15" t="s">
+      <c r="AJ5" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AK5" s="15" t="s">
+      <c r="AK5" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AL5" s="15" t="s">
+      <c r="AL5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AM5" s="15" t="s">
+      <c r="AM5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AN5" s="15" t="s">
+      <c r="AN5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AO5" s="15" t="s">
+      <c r="AO5" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="AP5" s="26" t="s">
+      <c r="AP5" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="AQ5" s="15" t="s">
+      <c r="AQ5" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AR5" s="15" t="s">
+      <c r="AR5" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AS5" s="15" t="s">
+      <c r="AS5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AT5" s="15" t="s">
+      <c r="AT5" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AU5" s="15" t="s">
+      <c r="AU5" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="AV5" s="15" t="s">
+      <c r="AV5" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AW5" s="15" t="s">
+      <c r="AW5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AX5" s="15" t="s">
+      <c r="AX5" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AY5" s="15" t="s">
+      <c r="AY5" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="AZ5" s="15" t="s">
+      <c r="AZ5" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="BA5" s="15" t="s">
+      <c r="BA5" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="BB5" s="15" t="s">
+      <c r="BB5" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="BC5" s="15" t="s">
+      <c r="BC5" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="BD5" s="15" t="s">
+      <c r="BD5" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="BE5" s="15" t="s">
+      <c r="BE5" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="BF5" s="15" t="s">
+      <c r="BF5" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="BG5" s="15" t="s">
+      <c r="BG5" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="BH5" s="15" t="s">
+      <c r="BH5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="BI5" s="15" t="s">
+      <c r="BI5" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="BJ5" s="15" t="s">
+      <c r="BJ5" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="BK5" s="15" t="s">
+      <c r="BK5" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="BL5" s="15" t="s">
+      <c r="BL5" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="BM5" s="15" t="s">
+      <c r="BM5" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="BN5" s="15" t="s">
+      <c r="BN5" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="BO5" s="15" t="s">
+      <c r="BO5" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="BP5" s="15" t="s">
+      <c r="BP5" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="AMJ5" s="25"/>
+      <c r="AMJ5" s="24"/>
     </row>
-    <row r="6" s="24" customFormat="true" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="n">
+    <row r="6" s="23" customFormat="true" ht="52.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="N6" s="15" t="n">
+      <c r="N6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="P6" s="15" t="n">
+      <c r="P6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="S6" s="15" t="n">
+      <c r="S6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="T6" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="U6" s="15" t="s">
+      <c r="U6" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="W6" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="X6" s="15" t="n">
+      <c r="X6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="Y6" s="15" t="s">
+      <c r="Y6" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="Z6" s="15" t="s">
+      <c r="Z6" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="AA6" s="15" t="s">
+      <c r="AA6" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AB6" s="15" t="n">
+      <c r="AB6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="AC6" s="18" t="s">
+      <c r="AC6" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AD6" s="18" t="s">
+      <c r="AD6" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AE6" s="18" t="n">
+      <c r="AE6" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="AF6" s="18" t="s">
+      <c r="AF6" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AG6" s="19" t="s">
+      <c r="AG6" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="AH6" s="19"/>
-      <c r="AI6" s="19" t="n">
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="18" t="n">
         <v>0.2</v>
       </c>
-      <c r="AJ6" s="19" t="n">
+      <c r="AJ6" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="AK6" s="19" t="n">
+      <c r="AK6" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="AL6" s="19" t="s">
+      <c r="AL6" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="AM6" s="19" t="s">
+      <c r="AM6" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="AN6" s="19" t="s">
+      <c r="AN6" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="AO6" s="19" t="n">
+      <c r="AO6" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="AP6" s="15" t="s">
+      <c r="AP6" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AQ6" s="15" t="n">
+      <c r="AQ6" s="14" t="n">
         <v>35</v>
       </c>
-      <c r="AR6" s="15" t="s">
+      <c r="AR6" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="AS6" s="20" t="s">
+      <c r="AS6" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AT6" s="20" t="s">
+      <c r="AT6" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AU6" s="21" t="e">
+      <c r="AU6" s="20" t="e">
         <f aca="false">IF(AQ6/(AR6-AT6/AS6*AR6)&gt;=1,1,AQ6/(AR6-AT6/AS6*AR6))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AV6" s="20" t="s">
+      <c r="AV6" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AW6" s="20" t="s">
+      <c r="AW6" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="AX6" s="18" t="s">
+      <c r="AX6" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AY6" s="15" t="s">
+      <c r="AY6" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="AZ6" s="15" t="s">
+      <c r="AZ6" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="BA6" s="15" t="s">
+      <c r="BA6" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="BB6" s="21" t="n">
+      <c r="BB6" s="20" t="n">
         <f aca="false">AO6+AK6+AE6+AB6+X6+S6+P6+N6</f>
         <v>8</v>
       </c>
-      <c r="BC6" s="21" t="n">
+      <c r="BC6" s="20" t="n">
         <v>100000</v>
       </c>
-      <c r="BD6" s="15" t="s">
+      <c r="BD6" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="BE6" s="21" t="s">
+      <c r="BE6" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="BF6" s="21" t="s">
+      <c r="BF6" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="BG6" s="15" t="s">
+      <c r="BG6" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="BH6" s="15" t="s">
+      <c r="BH6" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="BI6" s="15" t="s">
+      <c r="BI6" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="BJ6" s="15" t="s">
+      <c r="BJ6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="BK6" s="15" t="s">
+      <c r="BK6" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="BL6" s="15" t="s">
+      <c r="BL6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="BM6" s="22" t="s">
+      <c r="BM6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="BN6" s="18" t="s">
+      <c r="BN6" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="BO6" s="21" t="s">
+      <c r="BO6" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="BP6" s="18" t="s">
+      <c r="BP6" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="BQ6" s="23"/>
-      <c r="BR6" s="23"/>
-      <c r="BS6" s="23"/>
-      <c r="BT6" s="23"/>
-      <c r="BU6" s="23"/>
-      <c r="BV6" s="23"/>
-      <c r="BW6" s="23"/>
-      <c r="BX6" s="23"/>
-      <c r="BY6" s="23"/>
-      <c r="BZ6" s="23"/>
-      <c r="CA6" s="23"/>
-      <c r="CB6" s="23"/>
-      <c r="AMJ6" s="25"/>
+      <c r="BQ6" s="22"/>
+      <c r="BR6" s="22"/>
+      <c r="BS6" s="22"/>
+      <c r="BT6" s="22"/>
+      <c r="BU6" s="22"/>
+      <c r="BV6" s="22"/>
+      <c r="BW6" s="22"/>
+      <c r="BX6" s="22"/>
+      <c r="BY6" s="22"/>
+      <c r="BZ6" s="22"/>
+      <c r="CA6" s="22"/>
+      <c r="CB6" s="22"/>
+      <c r="AMJ6" s="24"/>
     </row>
-    <row r="7" s="15" customFormat="true" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+    <row r="7" s="14" customFormat="true" ht="52.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="Q7" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="R7" s="15" t="s">
+      <c r="R7" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="S7" s="15" t="s">
+      <c r="S7" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="T7" s="15" t="s">
+      <c r="T7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="U7" s="15" t="s">
+      <c r="U7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="V7" s="15" t="s">
+      <c r="V7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="W7" s="15" t="s">
+      <c r="W7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="X7" s="15" t="s">
+      <c r="X7" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="Y7" s="15" t="s">
+      <c r="Y7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="Z7" s="15" t="s">
+      <c r="Z7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AA7" s="15" t="s">
+      <c r="AA7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AB7" s="15" t="s">
+      <c r="AB7" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="AC7" s="15" t="s">
+      <c r="AC7" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AD7" s="15" t="s">
+      <c r="AD7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="AE7" s="15" t="s">
+      <c r="AE7" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="AF7" s="15" t="s">
+      <c r="AF7" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="AG7" s="15" t="s">
+      <c r="AG7" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="AH7" s="15" t="s">
+      <c r="AH7" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AI7" s="15" t="s">
+      <c r="AI7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AJ7" s="15" t="s">
+      <c r="AJ7" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AK7" s="15" t="s">
+      <c r="AK7" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AL7" s="15" t="s">
+      <c r="AL7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AM7" s="15" t="s">
+      <c r="AM7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AN7" s="15" t="s">
+      <c r="AN7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AO7" s="15" t="s">
+      <c r="AO7" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="AP7" s="15" t="s">
+      <c r="AP7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AQ7" s="15" t="s">
+      <c r="AQ7" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AR7" s="15" t="s">
+      <c r="AR7" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AS7" s="15" t="s">
+      <c r="AS7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AT7" s="15" t="s">
+      <c r="AT7" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AU7" s="15" t="s">
+      <c r="AU7" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="AV7" s="15" t="s">
+      <c r="AV7" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AW7" s="15" t="s">
+      <c r="AW7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AX7" s="15" t="s">
+      <c r="AX7" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AY7" s="15" t="s">
+      <c r="AY7" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="AZ7" s="15" t="s">
+      <c r="AZ7" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="BA7" s="15" t="s">
+      <c r="BA7" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="BB7" s="15" t="s">
+      <c r="BB7" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="BC7" s="15" t="s">
+      <c r="BC7" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="BD7" s="15" t="s">
+      <c r="BD7" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="BE7" s="15" t="s">
+      <c r="BE7" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="BF7" s="15" t="s">
+      <c r="BF7" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="BG7" s="15" t="s">
+      <c r="BG7" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="BH7" s="15" t="s">
+      <c r="BH7" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="BI7" s="15" t="s">
+      <c r="BI7" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="BJ7" s="15" t="s">
+      <c r="BJ7" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="BK7" s="15" t="s">
+      <c r="BK7" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="BL7" s="15" t="s">
+      <c r="BL7" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="BM7" s="15" t="s">
+      <c r="BM7" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="BN7" s="15" t="s">
+      <c r="BN7" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="BO7" s="27" t="s">
+      <c r="BO7" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="BP7" s="15" t="s">
+      <c r="BP7" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="AMJ7" s="25"/>
+      <c r="AMJ7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="54.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="54.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>